<commit_message>
update A lot of stuff
</commit_message>
<xml_diff>
--- a/Project Details/TestingPlan.xlsx
+++ b/Project Details/TestingPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21630" windowHeight="9975" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21630" windowHeight="9975"/>
   </bookViews>
   <sheets>
     <sheet name="5.1.1" sheetId="6" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="113">
   <si>
     <t>Test Case Name:</t>
   </si>
@@ -264,21 +264,9 @@
     <t>Verify that three units are communicating in an appropriate manner under various conditions.</t>
   </si>
   <si>
-    <t>South and West and East Unit Recieves North Unit Signal</t>
-  </si>
-  <si>
-    <t>North and West and East Unit Recieves South Unit Signal</t>
-  </si>
-  <si>
     <t>East Unit Sends a Signal</t>
   </si>
   <si>
-    <t>North and South and West Unit Recieves South Unit Signal</t>
-  </si>
-  <si>
-    <t>North and South and East Unit Recieves South Unit Signal</t>
-  </si>
-  <si>
     <t>Verify that four units are communicating in an appropriate manner under various conditions.</t>
   </si>
   <si>
@@ -321,19 +309,64 @@
     <t xml:space="preserve">Test module’s ability to both send and receive messages with no interference. </t>
   </si>
   <si>
-    <t>Serial Port ready message displayed</t>
-  </si>
-  <si>
-    <t>Start Arduino Tester software on Arduino</t>
-  </si>
-  <si>
-    <t>Begin Test</t>
-  </si>
-  <si>
-    <t>Connect Module to Arduino</t>
-  </si>
-  <si>
     <t>Test Writer:Max Cope</t>
+  </si>
+  <si>
+    <t>Module receives power and is on.</t>
+  </si>
+  <si>
+    <t>Serial Port "Ready" message displayed on screen.</t>
+  </si>
+  <si>
+    <t>Connect module two to Arduino two</t>
+  </si>
+  <si>
+    <t>Connect module one to Arduino two</t>
+  </si>
+  <si>
+    <t>Start Arduino tester software on Arduino one</t>
+  </si>
+  <si>
+    <t>Start Arduino tester software on Arduino two</t>
+  </si>
+  <si>
+    <t>Start test</t>
+  </si>
+  <si>
+    <t>Serial port "Ready" message displayed on screen.</t>
+  </si>
+  <si>
+    <t>Serial port should show a read out of the units "pinging" eachother and displaying timing results.</t>
+  </si>
+  <si>
+    <t>White Box</t>
+  </si>
+  <si>
+    <t>Power section on PCB should be set up with power supply attached and switch on</t>
+  </si>
+  <si>
+    <t>Board is fully powered on and IR unit is installed on the unit</t>
+  </si>
+  <si>
+    <t>Board is fully powered on and RF unit is installed on the unit</t>
+  </si>
+  <si>
+    <t>Two Arduino Unos are set up with RF test software loaded</t>
+  </si>
+  <si>
+    <t>Three powered-on units should be placed on opposite ends of a room from each other - maximum 100ft away from the farthest module. Each unit should be given a unique ID via the DIP switch.</t>
+  </si>
+  <si>
+    <t>South and West and East Unit Receives North Unit Signal</t>
+  </si>
+  <si>
+    <t>North and West and East Unit Receives South Unit Signal</t>
+  </si>
+  <si>
+    <t>North and South and East Unit Receives South Unit Signal</t>
+  </si>
+  <si>
+    <t>North and South and West Unit Receives South Unit Signal</t>
   </si>
 </sst>
 </file>
@@ -924,7 +957,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1059,6 +1092,13 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1277,14 +1317,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3022,8 +3054,8 @@
   </sheetPr>
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3033,6 +3065,7 @@
     <col min="3" max="3" width="33.85546875" customWidth="1"/>
     <col min="4" max="6" width="4" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3043,28 +3076,28 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="45"/>
-    </row>
-    <row r="3" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="46" t="s">
+      <c r="A2" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="47"/>
+    </row>
+    <row r="3" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="48" t="s">
+      <c r="B3" s="49"/>
+      <c r="C3" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="50"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="52"/>
       <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
@@ -3073,104 +3106,106 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="57" t="s">
+      <c r="B4" s="54"/>
+      <c r="C4" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="66" t="s">
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="8"/>
+      <c r="H4" s="8" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="67"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="69"/>
       <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="67"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="69"/>
       <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="55"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="68"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="70"/>
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="71"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="73"/>
     </row>
     <row r="9" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="74"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="76"/>
       <c r="G9" s="11" t="s">
         <v>13</v>
       </c>
       <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="77"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="79"/>
       <c r="G10" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="40" t="s">
+      <c r="B11" s="41"/>
+      <c r="C11" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="42"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="44"/>
     </row>
     <row r="12" spans="1:8" ht="33.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
@@ -3191,10 +3226,10 @@
       <c r="F12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="81" t="s">
+      <c r="G12" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="82"/>
+      <c r="H12" s="84"/>
     </row>
     <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
@@ -3209,8 +3244,8 @@
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="84"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="86"/>
     </row>
     <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A14" s="16">
@@ -3225,8 +3260,8 @@
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
-      <c r="G14" s="85"/>
-      <c r="H14" s="86"/>
+      <c r="G14" s="87"/>
+      <c r="H14" s="88"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
@@ -3235,8 +3270,8 @@
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
-      <c r="G15" s="85"/>
-      <c r="H15" s="86"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="88"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
@@ -3245,8 +3280,8 @@
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
-      <c r="G16" s="85"/>
-      <c r="H16" s="86"/>
+      <c r="G16" s="87"/>
+      <c r="H16" s="88"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="26"/>
@@ -3265,15 +3300,15 @@
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
       <c r="F18" s="19"/>
-      <c r="G18" s="87"/>
-      <c r="H18" s="88"/>
+      <c r="G18" s="89"/>
+      <c r="H18" s="90"/>
     </row>
     <row r="19" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="78" t="s">
+      <c r="A19" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="79"/>
-      <c r="C19" s="80"/>
+      <c r="B19" s="81"/>
+      <c r="C19" s="82"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="6"/>
@@ -3304,7 +3339,7 @@
     <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="93" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="90" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -3313,11 +3348,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3338,28 +3374,28 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="45"/>
+      <c r="A2" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="47"/>
     </row>
     <row r="3" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="48" t="s">
+      <c r="B3" s="49"/>
+      <c r="C3" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="50"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="52"/>
       <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
@@ -3368,17 +3404,17 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="57" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="66" t="s">
+      <c r="B4" s="54"/>
+      <c r="C4" s="59" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="68" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="8" t="s">
@@ -3386,88 +3422,88 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="67"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="69"/>
       <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="67"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="69"/>
       <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="55"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="68"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="70"/>
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="71"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="73"/>
     </row>
     <row r="9" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="74"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="76"/>
       <c r="G9" s="11" t="s">
         <v>13</v>
       </c>
       <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="77"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="79"/>
       <c r="G10" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="1:8" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="38" t="s">
+    <row r="11" spans="1:8" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="91" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="92"/>
-      <c r="E11" s="92"/>
-      <c r="F11" s="92"/>
-      <c r="G11" s="92"/>
-      <c r="H11" s="93"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="93" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="94"/>
+      <c r="E11" s="94"/>
+      <c r="F11" s="94"/>
+      <c r="G11" s="94"/>
+      <c r="H11" s="95"/>
     </row>
     <row r="12" spans="1:8" ht="33.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
@@ -3488,10 +3524,10 @@
       <c r="F12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="81" t="s">
+      <c r="G12" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="82"/>
+      <c r="H12" s="84"/>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
@@ -3501,13 +3537,13 @@
         <v>31</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="84"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="86"/>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A14" s="16">
@@ -3517,13 +3553,13 @@
         <v>61</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
-      <c r="G14" s="85"/>
-      <c r="H14" s="86"/>
+      <c r="G14" s="87"/>
+      <c r="H14" s="88"/>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A15" s="16">
@@ -3533,29 +3569,29 @@
         <v>70</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
-      <c r="G15" s="85"/>
-      <c r="H15" s="86"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="88"/>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A16" s="16">
         <v>4</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
-      <c r="G16" s="94"/>
-      <c r="H16" s="95"/>
+      <c r="G16" s="96"/>
+      <c r="H16" s="97"/>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A17" s="16">
@@ -3570,8 +3606,8 @@
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
-      <c r="G17" s="85"/>
-      <c r="H17" s="86"/>
+      <c r="G17" s="87"/>
+      <c r="H17" s="88"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="16">
@@ -3586,8 +3622,8 @@
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
-      <c r="G18" s="85"/>
-      <c r="H18" s="86"/>
+      <c r="G18" s="87"/>
+      <c r="H18" s="88"/>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A19" s="16">
@@ -3602,8 +3638,8 @@
       <c r="D19" s="36"/>
       <c r="E19" s="36"/>
       <c r="F19" s="36"/>
-      <c r="G19" s="96"/>
-      <c r="H19" s="97"/>
+      <c r="G19" s="98"/>
+      <c r="H19" s="99"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="16">
@@ -3618,8 +3654,8 @@
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
-      <c r="G20" s="85"/>
-      <c r="H20" s="86"/>
+      <c r="G20" s="87"/>
+      <c r="H20" s="88"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18"/>
@@ -3628,15 +3664,15 @@
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
-      <c r="G21" s="87"/>
-      <c r="H21" s="88"/>
+      <c r="G21" s="89"/>
+      <c r="H21" s="90"/>
     </row>
     <row r="22" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="78" t="s">
+      <c r="A22" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="79"/>
-      <c r="C22" s="80"/>
+      <c r="B22" s="81"/>
+      <c r="C22" s="82"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="6"/>
@@ -3671,7 +3707,7 @@
     <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="91" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -3680,11 +3716,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3694,6 +3731,7 @@
     <col min="3" max="3" width="33.85546875" customWidth="1"/>
     <col min="4" max="6" width="4" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3704,28 +3742,28 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="45"/>
-    </row>
-    <row r="3" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="46" t="s">
+      <c r="A2" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="47"/>
+    </row>
+    <row r="3" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="48" t="s">
+      <c r="B3" s="49"/>
+      <c r="C3" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="50"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="52"/>
       <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
@@ -3734,104 +3772,108 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="57" t="s">
+      <c r="B4" s="54"/>
+      <c r="C4" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="66" t="s">
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="8"/>
+      <c r="H4" s="8" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="67"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="69"/>
       <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="67"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="69"/>
       <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="55"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="68"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="70"/>
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="71"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="73"/>
     </row>
     <row r="9" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="74"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="76"/>
       <c r="G9" s="11" t="s">
         <v>13</v>
       </c>
       <c r="H9" s="12"/>
     </row>
-    <row r="10" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="38" t="s">
+    <row r="10" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="77"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="79"/>
       <c r="G10" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="38" t="s">
+    <row r="11" spans="1:8" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="42"/>
-    </row>
-    <row r="12" spans="1:8" ht="33.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="41"/>
+      <c r="C11" s="93" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="94"/>
+      <c r="E11" s="94"/>
+      <c r="F11" s="94"/>
+      <c r="G11" s="94"/>
+      <c r="H11" s="95"/>
+    </row>
+    <row r="12" spans="1:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>5</v>
       </c>
@@ -3850,10 +3892,10 @@
       <c r="F12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="81" t="s">
+      <c r="G12" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="82"/>
+      <c r="H12" s="84"/>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
@@ -3868,8 +3910,8 @@
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
-      <c r="G13" s="85"/>
-      <c r="H13" s="86"/>
+      <c r="G13" s="87"/>
+      <c r="H13" s="88"/>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A14" s="16">
@@ -3884,8 +3926,8 @@
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
-      <c r="G14" s="85"/>
-      <c r="H14" s="86"/>
+      <c r="G14" s="87"/>
+      <c r="H14" s="88"/>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A15" s="16">
@@ -3900,8 +3942,8 @@
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
-      <c r="G15" s="85"/>
-      <c r="H15" s="86"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="88"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
@@ -3920,15 +3962,15 @@
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
       <c r="F17" s="19"/>
-      <c r="G17" s="87"/>
-      <c r="H17" s="88"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="90"/>
     </row>
     <row r="18" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="78" t="s">
+      <c r="A18" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="79"/>
-      <c r="C18" s="80"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="82"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="6"/>
@@ -3958,7 +4000,7 @@
     <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="90" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -3967,11 +4009,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="A13:C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3981,6 +4024,7 @@
     <col min="3" max="3" width="33.85546875" customWidth="1"/>
     <col min="4" max="6" width="4" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3991,28 +4035,28 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="45"/>
-    </row>
-    <row r="3" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="46" t="s">
+      <c r="A2" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="47"/>
+    </row>
+    <row r="3" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="48" t="s">
+      <c r="B3" s="49"/>
+      <c r="C3" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="50"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="52"/>
       <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
@@ -4021,102 +4065,106 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="57" t="s">
+      <c r="B4" s="54"/>
+      <c r="C4" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="66" t="s">
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="8"/>
+      <c r="H4" s="8" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="67"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="69"/>
       <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="67"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="69"/>
       <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="55"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="68"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="70"/>
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="71"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="73"/>
     </row>
     <row r="9" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="74"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="76"/>
       <c r="G9" s="11" t="s">
         <v>13</v>
       </c>
       <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="77"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="79"/>
       <c r="G10" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="42"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="44"/>
     </row>
     <row r="12" spans="1:8" ht="33.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
@@ -4137,10 +4185,10 @@
       <c r="F12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="81" t="s">
+      <c r="G12" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="82"/>
+      <c r="H12" s="84"/>
     </row>
     <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
@@ -4155,8 +4203,8 @@
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="84"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="86"/>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A14" s="16">
@@ -4171,8 +4219,8 @@
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
-      <c r="G14" s="85"/>
-      <c r="H14" s="86"/>
+      <c r="G14" s="87"/>
+      <c r="H14" s="88"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
@@ -4181,8 +4229,8 @@
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
-      <c r="G15" s="89"/>
-      <c r="H15" s="90"/>
+      <c r="G15" s="91"/>
+      <c r="H15" s="92"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
@@ -4191,8 +4239,8 @@
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
-      <c r="G16" s="85"/>
-      <c r="H16" s="86"/>
+      <c r="G16" s="87"/>
+      <c r="H16" s="88"/>
     </row>
     <row r="17" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="18"/>
@@ -4201,15 +4249,15 @@
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
       <c r="F17" s="19"/>
-      <c r="G17" s="87"/>
-      <c r="H17" s="88"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="90"/>
     </row>
     <row r="18" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="78" t="s">
+      <c r="A18" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="79"/>
-      <c r="C18" s="80"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="82"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="6"/>
@@ -4240,7 +4288,7 @@
     <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="90" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -4249,11 +4297,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4263,6 +4312,7 @@
     <col min="3" max="3" width="33.85546875" customWidth="1"/>
     <col min="4" max="6" width="4" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4273,28 +4323,28 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="45"/>
-    </row>
-    <row r="3" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="46" t="s">
+      <c r="A2" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="47"/>
+    </row>
+    <row r="3" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="48" t="s">
+      <c r="B3" s="49"/>
+      <c r="C3" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="50"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="52"/>
       <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
@@ -4303,102 +4353,106 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="57" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="66" t="s">
+      <c r="B4" s="54"/>
+      <c r="C4" s="59" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="8"/>
+      <c r="H4" s="8" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="67"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="69"/>
       <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="67"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="69"/>
       <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="55"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="68"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="70"/>
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="71"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="73"/>
     </row>
     <row r="9" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="74"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="76"/>
       <c r="G9" s="11" t="s">
         <v>13</v>
       </c>
       <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="77"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="79"/>
       <c r="G10" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="42"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="44"/>
     </row>
     <row r="12" spans="1:8" ht="33.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
@@ -4419,42 +4473,42 @@
       <c r="F12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="81" t="s">
+      <c r="G12" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="82"/>
+      <c r="H12" s="84"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
         <v>1</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="84"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="86"/>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A14" s="16">
         <v>2</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
-      <c r="G14" s="85"/>
-      <c r="H14" s="86"/>
+      <c r="G14" s="87"/>
+      <c r="H14" s="88"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
@@ -4463,8 +4517,8 @@
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
-      <c r="G15" s="85"/>
-      <c r="H15" s="86"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="88"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
@@ -4473,8 +4527,8 @@
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
-      <c r="G16" s="85"/>
-      <c r="H16" s="86"/>
+      <c r="G16" s="87"/>
+      <c r="H16" s="88"/>
     </row>
     <row r="17" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="18"/>
@@ -4483,15 +4537,15 @@
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
       <c r="F17" s="19"/>
-      <c r="G17" s="87"/>
-      <c r="H17" s="88"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="90"/>
     </row>
     <row r="18" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="78" t="s">
+      <c r="A18" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="79"/>
-      <c r="C18" s="80"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="82"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="6"/>
@@ -4522,7 +4576,7 @@
     <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="90" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -4531,11 +4585,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4545,6 +4600,7 @@
     <col min="3" max="3" width="33.85546875" customWidth="1"/>
     <col min="4" max="6" width="4" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4555,28 +4611,28 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="43" t="s">
-        <v>101</v>
-      </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="45"/>
+      <c r="A2" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="47"/>
     </row>
     <row r="3" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="48" t="s">
-        <v>92</v>
-      </c>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="50"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="52"/>
       <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
@@ -4585,102 +4641,106 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="57" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="66" t="s">
+      <c r="B4" s="54"/>
+      <c r="C4" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="8"/>
+      <c r="H4" s="8" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="67"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="69"/>
       <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="67"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="69"/>
       <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="55"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="68"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="70"/>
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="71"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="73"/>
     </row>
     <row r="9" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="74"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="76"/>
       <c r="G9" s="11" t="s">
         <v>13</v>
       </c>
       <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="77"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="79"/>
       <c r="G10" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="42"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="44"/>
     </row>
     <row r="12" spans="1:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
@@ -4701,10 +4761,10 @@
       <c r="F12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="81" t="s">
+      <c r="G12" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="82"/>
+      <c r="H12" s="84"/>
     </row>
     <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
@@ -4714,20 +4774,20 @@
         <v>56</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="84"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="86"/>
     </row>
     <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
         <v>2</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C14" s="35" t="s">
         <v>59</v>
@@ -4735,8 +4795,8 @@
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
-      <c r="G14" s="85"/>
-      <c r="H14" s="86"/>
+      <c r="G14" s="87"/>
+      <c r="H14" s="88"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
@@ -4745,8 +4805,8 @@
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
-      <c r="G15" s="85"/>
-      <c r="H15" s="86"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="88"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
@@ -4755,8 +4815,8 @@
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
-      <c r="G16" s="85"/>
-      <c r="H16" s="86"/>
+      <c r="G16" s="87"/>
+      <c r="H16" s="88"/>
     </row>
     <row r="17" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="18"/>
@@ -4765,15 +4825,15 @@
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
       <c r="F17" s="19"/>
-      <c r="G17" s="87"/>
-      <c r="H17" s="88"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="90"/>
     </row>
     <row r="18" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="78" t="s">
+      <c r="A18" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="79"/>
-      <c r="C18" s="80"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="82"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="6"/>
@@ -4804,7 +4864,7 @@
     <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="90" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -4812,12 +4872,13 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
+    <tabColor rgb="FF00B050"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4827,6 +4888,7 @@
     <col min="3" max="3" width="33.85546875" customWidth="1"/>
     <col min="4" max="6" width="4" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4837,28 +4899,28 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="43" t="s">
-        <v>101</v>
-      </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="45"/>
+      <c r="A2" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="47"/>
     </row>
     <row r="3" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="50"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="52"/>
       <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
@@ -4867,102 +4929,106 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="57" t="s">
-        <v>96</v>
-      </c>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="66" t="s">
+      <c r="B4" s="54"/>
+      <c r="C4" s="59" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="8"/>
+      <c r="H4" s="8" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="67"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="69"/>
       <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="67"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="69"/>
       <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="55"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="68"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="70"/>
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="71"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="73"/>
     </row>
     <row r="9" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="74"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="76"/>
       <c r="G9" s="11" t="s">
         <v>13</v>
       </c>
       <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="77"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="79"/>
       <c r="G10" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="42"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="44"/>
     </row>
     <row r="12" spans="1:8" ht="36" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
@@ -4983,83 +5049,97 @@
       <c r="F12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="81" t="s">
+      <c r="G12" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="82"/>
+      <c r="H12" s="84"/>
     </row>
     <row r="13" spans="1:8" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>1</v>
       </c>
-      <c r="B13" s="100" t="s">
-        <v>100</v>
-      </c>
-      <c r="C13" s="99"/>
+      <c r="B13" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>94</v>
+      </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="84"/>
-    </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G13" s="85"/>
+      <c r="H13" s="86"/>
+    </row>
+    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
         <v>2</v>
       </c>
-      <c r="B14" s="98" t="s">
+      <c r="B14" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="C14" s="98" t="s">
-        <v>97</v>
+      <c r="C14" s="38" t="s">
+        <v>95</v>
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
-      <c r="G14" s="85"/>
-      <c r="H14" s="86"/>
-    </row>
-    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="G14" s="87"/>
+      <c r="H14" s="88"/>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
         <v>3</v>
       </c>
       <c r="B15" s="35" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
-      <c r="G15" s="85"/>
-      <c r="H15" s="86"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="88"/>
+    </row>
+    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="16">
+        <v>4</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>101</v>
+      </c>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
-      <c r="G16" s="85"/>
-      <c r="H16" s="86"/>
-    </row>
-    <row r="17" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="18"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
+      <c r="G16" s="87"/>
+      <c r="H16" s="88"/>
+    </row>
+    <row r="17" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="18">
+        <v>5</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>102</v>
+      </c>
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
       <c r="F17" s="19"/>
-      <c r="G17" s="87"/>
-      <c r="H17" s="88"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="90"/>
     </row>
     <row r="18" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="78" t="s">
+      <c r="A18" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="79"/>
-      <c r="C18" s="80"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="82"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="6"/>
@@ -5090,7 +5170,7 @@
     <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="90" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -5099,11 +5179,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5113,6 +5194,7 @@
     <col min="3" max="3" width="33.85546875" customWidth="1"/>
     <col min="4" max="6" width="4" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5123,28 +5205,28 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="45"/>
+      <c r="A2" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="47"/>
     </row>
     <row r="3" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="48" t="s">
+      <c r="B3" s="49"/>
+      <c r="C3" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="50"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="52"/>
       <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
@@ -5153,104 +5235,106 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="57" t="s">
+      <c r="B4" s="54"/>
+      <c r="C4" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="66" t="s">
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="8"/>
+      <c r="H4" s="8" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="67"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="69"/>
       <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="67"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="69"/>
       <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="55"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="68"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="70"/>
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="71"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="73"/>
     </row>
     <row r="9" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="74"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="76"/>
       <c r="G9" s="11" t="s">
         <v>13</v>
       </c>
       <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="77"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="79"/>
       <c r="G10" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="40" t="s">
+      <c r="B11" s="41"/>
+      <c r="C11" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="42"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="44"/>
     </row>
     <row r="12" spans="1:8" ht="33.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
@@ -5271,10 +5355,10 @@
       <c r="F12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="81" t="s">
+      <c r="G12" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="82"/>
+      <c r="H12" s="84"/>
     </row>
     <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
@@ -5289,8 +5373,8 @@
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="84"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="86"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
@@ -5299,8 +5383,8 @@
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
-      <c r="G14" s="85"/>
-      <c r="H14" s="86"/>
+      <c r="G14" s="87"/>
+      <c r="H14" s="88"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
@@ -5309,8 +5393,8 @@
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
-      <c r="G15" s="85"/>
-      <c r="H15" s="86"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="88"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
@@ -5319,8 +5403,8 @@
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
-      <c r="G16" s="85"/>
-      <c r="H16" s="86"/>
+      <c r="G16" s="87"/>
+      <c r="H16" s="88"/>
     </row>
     <row r="17" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="18"/>
@@ -5329,15 +5413,15 @@
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
       <c r="F17" s="19"/>
-      <c r="G17" s="87"/>
-      <c r="H17" s="88"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="90"/>
     </row>
     <row r="18" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="78" t="s">
+      <c r="A18" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="79"/>
-      <c r="C18" s="80"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="82"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="6"/>
@@ -5368,7 +5452,7 @@
     <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="90" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -5377,11 +5461,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5402,28 +5487,28 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="45"/>
+      <c r="A2" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="47"/>
     </row>
     <row r="3" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="48" t="s">
+      <c r="B3" s="49"/>
+      <c r="C3" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="50"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="52"/>
       <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
@@ -5432,17 +5517,17 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="57" t="s">
+      <c r="B4" s="54"/>
+      <c r="C4" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="66" t="s">
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="68" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="8" t="s">
@@ -5450,88 +5535,88 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="67"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="69"/>
       <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="67"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="69"/>
       <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="55"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="68"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="70"/>
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="71"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="73"/>
     </row>
     <row r="9" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="74"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="76"/>
       <c r="G9" s="11" t="s">
         <v>13</v>
       </c>
       <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="77"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="79"/>
       <c r="G10" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="91" t="s">
+      <c r="B11" s="41"/>
+      <c r="C11" s="93" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="92"/>
-      <c r="E11" s="92"/>
-      <c r="F11" s="92"/>
-      <c r="G11" s="92"/>
-      <c r="H11" s="93"/>
+      <c r="D11" s="94"/>
+      <c r="E11" s="94"/>
+      <c r="F11" s="94"/>
+      <c r="G11" s="94"/>
+      <c r="H11" s="95"/>
     </row>
     <row r="12" spans="1:8" ht="33.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
@@ -5552,10 +5637,10 @@
       <c r="F12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="81" t="s">
+      <c r="G12" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="82"/>
+      <c r="H12" s="84"/>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
@@ -5570,8 +5655,8 @@
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="84"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="86"/>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A14" s="16">
@@ -5586,8 +5671,8 @@
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
-      <c r="G14" s="85"/>
-      <c r="H14" s="86"/>
+      <c r="G14" s="87"/>
+      <c r="H14" s="88"/>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A15" s="16">
@@ -5602,8 +5687,8 @@
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
-      <c r="G15" s="85"/>
-      <c r="H15" s="86"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="88"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="16">
@@ -5634,8 +5719,8 @@
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
-      <c r="G17" s="85"/>
-      <c r="H17" s="86"/>
+      <c r="G17" s="87"/>
+      <c r="H17" s="88"/>
     </row>
     <row r="18" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="18">
@@ -5650,15 +5735,15 @@
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
       <c r="F18" s="19"/>
-      <c r="G18" s="87"/>
-      <c r="H18" s="88"/>
+      <c r="G18" s="89"/>
+      <c r="H18" s="90"/>
     </row>
     <row r="19" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="78" t="s">
+      <c r="A19" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="79"/>
-      <c r="C19" s="80"/>
+      <c r="B19" s="81"/>
+      <c r="C19" s="82"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="6"/>
@@ -5667,6 +5752,17 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F7"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="C9:F9"/>
@@ -5676,20 +5772,9 @@
     <mergeCell ref="G4:G7"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C4:F7"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="C11:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="91" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -5698,11 +5783,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5723,28 +5809,28 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="45"/>
+      <c r="A2" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="47"/>
     </row>
     <row r="3" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="48" t="s">
+      <c r="B3" s="49"/>
+      <c r="C3" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="50"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="52"/>
       <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
@@ -5753,17 +5839,17 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="57" t="s">
+      <c r="B4" s="54"/>
+      <c r="C4" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="66" t="s">
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="68" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="8" t="s">
@@ -5771,88 +5857,88 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="67"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="69"/>
       <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="67"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="69"/>
       <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="55"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="68"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="70"/>
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="71"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="73"/>
     </row>
     <row r="9" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="74"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="76"/>
       <c r="G9" s="11" t="s">
         <v>13</v>
       </c>
       <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="77"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="79"/>
       <c r="G10" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="91" t="s">
+      <c r="B11" s="41"/>
+      <c r="C11" s="93" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="92"/>
-      <c r="E11" s="92"/>
-      <c r="F11" s="92"/>
-      <c r="G11" s="92"/>
-      <c r="H11" s="93"/>
+      <c r="D11" s="94"/>
+      <c r="E11" s="94"/>
+      <c r="F11" s="94"/>
+      <c r="G11" s="94"/>
+      <c r="H11" s="95"/>
     </row>
     <row r="12" spans="1:8" ht="33.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
@@ -5873,10 +5959,10 @@
       <c r="F12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="81" t="s">
+      <c r="G12" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="82"/>
+      <c r="H12" s="84"/>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
@@ -5891,8 +5977,8 @@
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="84"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="86"/>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A14" s="16">
@@ -5907,8 +5993,8 @@
       <c r="D14" s="36"/>
       <c r="E14" s="36"/>
       <c r="F14" s="36"/>
-      <c r="G14" s="94"/>
-      <c r="H14" s="95"/>
+      <c r="G14" s="96"/>
+      <c r="H14" s="97"/>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A15" s="16">
@@ -5923,8 +6009,8 @@
       <c r="D15" s="36"/>
       <c r="E15" s="36"/>
       <c r="F15" s="36"/>
-      <c r="G15" s="94"/>
-      <c r="H15" s="95"/>
+      <c r="G15" s="96"/>
+      <c r="H15" s="97"/>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A16" s="16">
@@ -5939,8 +6025,8 @@
       <c r="D16" s="36"/>
       <c r="E16" s="36"/>
       <c r="F16" s="36"/>
-      <c r="G16" s="94"/>
-      <c r="H16" s="95"/>
+      <c r="G16" s="96"/>
+      <c r="H16" s="97"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="16">
@@ -5955,8 +6041,8 @@
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
-      <c r="G17" s="85"/>
-      <c r="H17" s="86"/>
+      <c r="G17" s="87"/>
+      <c r="H17" s="88"/>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A18" s="16">
@@ -5971,8 +6057,8 @@
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
-      <c r="G18" s="85"/>
-      <c r="H18" s="86"/>
+      <c r="G18" s="87"/>
+      <c r="H18" s="88"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="16">
@@ -5987,8 +6073,8 @@
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
-      <c r="G19" s="85"/>
-      <c r="H19" s="86"/>
+      <c r="G19" s="87"/>
+      <c r="H19" s="88"/>
     </row>
     <row r="20" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="31"/>
@@ -5997,15 +6083,15 @@
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
       <c r="F20" s="19"/>
-      <c r="G20" s="87"/>
-      <c r="H20" s="88"/>
+      <c r="G20" s="89"/>
+      <c r="H20" s="90"/>
     </row>
     <row r="21" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="78" t="s">
+      <c r="A21" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="79"/>
-      <c r="C21" s="80"/>
+      <c r="B21" s="81"/>
+      <c r="C21" s="82"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="6"/>
@@ -6039,7 +6125,7 @@
     <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="91" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>